<commit_message>
Update template to include 2.11 updates
</commit_message>
<xml_diff>
--- a/template-generator/USDM_2.11_Test_Data_Template.xlsx
+++ b/template-generator/USDM_2.11_Test_Data_Template.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1890">
   <si>
     <t>Filename</t>
   </si>
@@ -3455,13 +3455,16 @@
     <t>Section Title</t>
   </si>
   <si>
-    <t>(Narrative Content Previous) [Identifiers][Any Exist]</t>
-  </si>
-  <si>
-    <t>(Narrative Content Next) [Identifiers][Any Exist]</t>
+    <t>(Narrative Content Previous) [Identifier]</t>
+  </si>
+  <si>
+    <t>(Narrative Content Next) [Identifier]</t>
   </si>
   <si>
     <t>(Narrative Content Children) [Identifiers][Any Exist]</t>
+  </si>
+  <si>
+    <t>NarrativeContent[0..1].id[1]</t>
   </si>
   <si>
     <t>NarrativeContent[0..*].id[1]</t>
@@ -6513,299 +6516,299 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B36" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C36" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B37" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C37" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="B38" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="C38" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B39" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="C39" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B40" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="C40" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="B41" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="C41" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="B42" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="C42" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="B43" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="C43" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="B44" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="C44" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="B45" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="C45" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="B46" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="C46" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="B47" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="C47" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="B48" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="C48" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="B49" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="C49" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B50" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="C50" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B51" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="C51" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="B52" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="C52" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B53" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="C53" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B54" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="C54" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="B55" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="C55" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="B56" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="C56" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="B57" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="C57" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
       <c r="B58" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="C58" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="B59" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="C59" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="B60" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="C60" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="B61" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
       <c r="C61" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="B62" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="C62" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
     </row>
   </sheetData>
@@ -13397,10 +13400,10 @@
         <v>38</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>39</v>
@@ -13444,7 +13447,7 @@
         <v>1129</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -13507,7 +13510,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -13524,22 +13527,22 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13603,7 +13606,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -13675,25 +13678,25 @@
         <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>660</v>
@@ -13716,58 +13719,58 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -13897,13 +13900,13 @@
         <v>77</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -13972,7 +13975,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -13996,7 +13999,7 @@
         <v>635</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -14013,43 +14016,43 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14078,7 +14081,7 @@
         <v>38</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>38</v>
@@ -14155,7 +14158,7 @@
         <v>77</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -14210,7 +14213,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -14248,31 +14251,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -14860,52 +14863,52 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>659</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -14922,55 +14925,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -15067,40 +15070,40 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -15188,22 +15191,22 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15267,7 +15270,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -15315,7 +15318,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>230</v>
@@ -15324,70 +15327,70 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>263</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -15404,82 +15407,82 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -15651,19 +15654,19 @@
         <v>78</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="AC4" s="3" t="s">
         <v>420</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -15793,55 +15796,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -16081,40 +16084,40 @@
         <v>14</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2" spans="1:34">
@@ -16131,94 +16134,94 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -16393,40 +16396,40 @@
         <v>40</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -16510,7 +16513,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>630</v>
@@ -16531,97 +16534,97 @@
         <v>635</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>452</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2" spans="1:47">
@@ -16638,133 +16641,133 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="3" spans="1:47">
@@ -16939,7 +16942,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>72</v>
@@ -17017,40 +17020,40 @@
         <v>403</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="5" spans="1:47">
@@ -17138,49 +17141,49 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -17197,55 +17200,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -17342,40 +17345,40 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -17446,145 +17449,145 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:56">
@@ -17601,160 +17604,160 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="3" spans="1:56">
@@ -17956,55 +17959,55 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>937</v>
@@ -18034,40 +18037,40 @@
         <v>945</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="AV4" s="3" t="s">
         <v>937</v>
@@ -18194,31 +18197,31 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -18235,40 +18238,40 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -18577,148 +18580,148 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="3" spans="1:52">
@@ -19034,7 +19037,7 @@
         <v>40</v>
       </c>
       <c r="AZ4" s="3" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -19575,25 +19578,25 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>30</v>
@@ -19722,34 +19725,34 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -19766,37 +19769,37 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -19981,31 +19984,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -20159,10 +20162,10 @@
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -20179,34 +20182,34 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -20291,10 +20294,10 @@
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -20352,22 +20355,22 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -20384,31 +20387,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -20619,7 +20622,7 @@
         <v>14</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -20636,64 +20639,64 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>207</v>
@@ -20717,7 +20720,7 @@
         <v>30</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -20913,7 +20916,7 @@
         <v>40</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1766</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -20995,91 +20998,91 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1786</v>
+        <v>1787</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1788</v>
+        <v>1789</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1789</v>
+        <v>1790</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1791</v>
+        <v>1792</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1794</v>
+        <v>1795</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1796</v>
+        <v>1797</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1797</v>
+        <v>1798</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -21096,106 +21099,106 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1801</v>
+        <v>1802</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1802</v>
+        <v>1803</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1805</v>
+        <v>1806</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1809</v>
+        <v>1810</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1814</v>
+        <v>1815</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -21343,91 +21346,91 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -21503,7 +21506,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>912</v>
@@ -21526,13 +21529,13 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
@@ -21552,7 +21555,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
@@ -21633,13 +21636,13 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -21656,16 +21659,16 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -21682,7 +21685,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
@@ -21777,7 +21780,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23090,7 +23093,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23181,7 +23184,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23272,7 +23275,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>

<commit_message>
Update template with model changes
</commit_message>
<xml_diff>
--- a/template-generator/USDM_2.11_Test_Data_Template.xlsx
+++ b/template-generator/USDM_2.11_Test_Data_Template.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1890">
   <si>
     <t>Filename</t>
   </si>
@@ -3455,13 +3455,16 @@
     <t>Section Title</t>
   </si>
   <si>
-    <t>(Narrative Content Previous) [Identifiers][Any Exist]</t>
-  </si>
-  <si>
-    <t>(Narrative Content Next) [Identifiers][Any Exist]</t>
+    <t>(Narrative Content Previous) [Identifier]</t>
+  </si>
+  <si>
+    <t>(Narrative Content Next) [Identifier]</t>
   </si>
   <si>
     <t>(Narrative Content Children) [Identifiers][Any Exist]</t>
+  </si>
+  <si>
+    <t>NarrativeContent[0..1].id[1]</t>
   </si>
   <si>
     <t>NarrativeContent[0..*].id[1]</t>
@@ -6513,299 +6516,299 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B36" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C36" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B37" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C37" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="B38" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="C38" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B39" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="C39" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B40" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="C40" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="B41" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="C41" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="B42" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="C42" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="B43" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="C43" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="B44" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="C44" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="B45" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="C45" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="B46" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="C46" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="B47" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="C47" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="B48" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="C48" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="B49" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="C49" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B50" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="C50" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B51" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="C51" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="B52" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="C52" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B53" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="C53" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B54" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="C54" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="B55" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="C55" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="B56" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="C56" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="B57" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="C57" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
       <c r="B58" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="C58" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="B59" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="C59" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="B60" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="C60" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="B61" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
       <c r="C61" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="B62" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="C62" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
     </row>
   </sheetData>
@@ -13397,10 +13400,10 @@
         <v>38</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>39</v>
@@ -13444,7 +13447,7 @@
         <v>1129</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -13507,7 +13510,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -13524,22 +13527,22 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13603,7 +13606,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -13675,25 +13678,25 @@
         <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>660</v>
@@ -13716,58 +13719,58 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -13897,13 +13900,13 @@
         <v>77</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -13972,7 +13975,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -13996,7 +13999,7 @@
         <v>635</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -14013,43 +14016,43 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14078,7 +14081,7 @@
         <v>38</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>38</v>
@@ -14155,7 +14158,7 @@
         <v>77</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -14210,7 +14213,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -14248,31 +14251,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -14860,52 +14863,52 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>659</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -14922,55 +14925,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -15067,40 +15070,40 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -15188,22 +15191,22 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15267,7 +15270,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -15315,7 +15318,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>230</v>
@@ -15324,70 +15327,70 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>263</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -15404,82 +15407,82 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -15651,19 +15654,19 @@
         <v>78</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="AC4" s="3" t="s">
         <v>420</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -15793,55 +15796,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -16081,40 +16084,40 @@
         <v>14</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2" spans="1:34">
@@ -16131,94 +16134,94 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -16393,40 +16396,40 @@
         <v>40</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -16510,7 +16513,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>630</v>
@@ -16531,97 +16534,97 @@
         <v>635</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>452</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2" spans="1:47">
@@ -16638,133 +16641,133 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="3" spans="1:47">
@@ -16939,7 +16942,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>72</v>
@@ -17017,40 +17020,40 @@
         <v>403</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="5" spans="1:47">
@@ -17138,49 +17141,49 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -17197,55 +17200,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -17342,40 +17345,40 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -17446,145 +17449,145 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:56">
@@ -17601,160 +17604,160 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="3" spans="1:56">
@@ -17956,55 +17959,55 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>937</v>
@@ -18034,40 +18037,40 @@
         <v>945</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="AV4" s="3" t="s">
         <v>937</v>
@@ -18194,31 +18197,31 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -18235,40 +18238,40 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -18577,148 +18580,148 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="3" spans="1:52">
@@ -19034,7 +19037,7 @@
         <v>40</v>
       </c>
       <c r="AZ4" s="3" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -19575,25 +19578,25 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>30</v>
@@ -19722,34 +19725,34 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -19766,37 +19769,37 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -19981,31 +19984,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -20159,10 +20162,10 @@
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -20179,34 +20182,34 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -20291,10 +20294,10 @@
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -20352,22 +20355,22 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -20384,31 +20387,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -20619,7 +20622,7 @@
         <v>14</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -20636,64 +20639,64 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>207</v>
@@ -20717,7 +20720,7 @@
         <v>30</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -20913,7 +20916,7 @@
         <v>40</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1766</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -20995,91 +20998,91 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1786</v>
+        <v>1787</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1788</v>
+        <v>1789</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1789</v>
+        <v>1790</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1791</v>
+        <v>1792</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1794</v>
+        <v>1795</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1796</v>
+        <v>1797</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1797</v>
+        <v>1798</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -21096,106 +21099,106 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1801</v>
+        <v>1802</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1802</v>
+        <v>1803</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1805</v>
+        <v>1806</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1809</v>
+        <v>1810</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1814</v>
+        <v>1815</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -21343,91 +21346,91 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -21503,7 +21506,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>912</v>
@@ -21526,13 +21529,13 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
@@ -21552,7 +21555,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
@@ -21633,13 +21636,13 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -21656,16 +21659,16 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -21682,7 +21685,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
@@ -21777,7 +21780,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23090,7 +23093,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23181,7 +23184,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23272,7 +23275,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>

<commit_message>
Update template with model changes (#171)
</commit_message>
<xml_diff>
--- a/template-generator/USDM_2.11_Test_Data_Template.xlsx
+++ b/template-generator/USDM_2.11_Test_Data_Template.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1890">
   <si>
     <t>Filename</t>
   </si>
@@ -3455,13 +3455,16 @@
     <t>Section Title</t>
   </si>
   <si>
-    <t>(Narrative Content Previous) [Identifiers][Any Exist]</t>
-  </si>
-  <si>
-    <t>(Narrative Content Next) [Identifiers][Any Exist]</t>
+    <t>(Narrative Content Previous) [Identifier]</t>
+  </si>
+  <si>
+    <t>(Narrative Content Next) [Identifier]</t>
   </si>
   <si>
     <t>(Narrative Content Children) [Identifiers][Any Exist]</t>
+  </si>
+  <si>
+    <t>NarrativeContent[0..1].id[1]</t>
   </si>
   <si>
     <t>NarrativeContent[0..*].id[1]</t>
@@ -6513,299 +6516,299 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B36" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C36" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B37" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C37" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="B38" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="C38" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B39" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="C39" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B40" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="C40" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="B41" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="C41" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="B42" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="C42" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="B43" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="C43" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="B44" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="C44" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="B45" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="C45" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="B46" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="C46" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="B47" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="C47" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="B48" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="C48" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="B49" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="C49" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B50" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="C50" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B51" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="C51" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="B52" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="C52" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B53" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="C53" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B54" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="C54" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="B55" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="C55" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="B56" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="C56" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="B57" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="C57" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
       <c r="B58" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="C58" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="B59" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="C59" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="B60" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="C60" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="B61" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
       <c r="C61" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="B62" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="C62" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
     </row>
   </sheetData>
@@ -13397,10 +13400,10 @@
         <v>38</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>39</v>
@@ -13444,7 +13447,7 @@
         <v>1129</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -13507,7 +13510,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -13524,22 +13527,22 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13603,7 +13606,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -13675,25 +13678,25 @@
         <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>660</v>
@@ -13716,58 +13719,58 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -13897,13 +13900,13 @@
         <v>77</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -13972,7 +13975,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -13996,7 +13999,7 @@
         <v>635</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -14013,43 +14016,43 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14078,7 +14081,7 @@
         <v>38</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>38</v>
@@ -14155,7 +14158,7 @@
         <v>77</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -14210,7 +14213,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -14248,31 +14251,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -14860,52 +14863,52 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>659</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -14922,55 +14925,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -15067,40 +15070,40 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -15188,22 +15191,22 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -15267,7 +15270,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -15315,7 +15318,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>230</v>
@@ -15324,70 +15327,70 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>263</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -15404,82 +15407,82 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -15651,19 +15654,19 @@
         <v>78</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="AC4" s="3" t="s">
         <v>420</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -15793,55 +15796,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -16081,40 +16084,40 @@
         <v>14</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2" spans="1:34">
@@ -16131,94 +16134,94 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -16393,40 +16396,40 @@
         <v>40</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -16510,7 +16513,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>630</v>
@@ -16531,97 +16534,97 @@
         <v>635</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>452</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2" spans="1:47">
@@ -16638,133 +16641,133 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="3" spans="1:47">
@@ -16939,7 +16942,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>72</v>
@@ -17017,40 +17020,40 @@
         <v>403</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="5" spans="1:47">
@@ -17138,49 +17141,49 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -17197,55 +17200,55 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -17342,40 +17345,40 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -17446,145 +17449,145 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:56">
@@ -17601,160 +17604,160 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="3" spans="1:56">
@@ -17956,55 +17959,55 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>937</v>
@@ -18034,40 +18037,40 @@
         <v>945</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="AV4" s="3" t="s">
         <v>937</v>
@@ -18194,31 +18197,31 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -18235,40 +18238,40 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -18577,148 +18580,148 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="3" spans="1:52">
@@ -19034,7 +19037,7 @@
         <v>40</v>
       </c>
       <c r="AZ4" s="3" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -19575,25 +19578,25 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>30</v>
@@ -19722,34 +19725,34 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -19766,37 +19769,37 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -19981,31 +19984,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -20159,10 +20162,10 @@
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -20179,34 +20182,34 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -20291,10 +20294,10 @@
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -20352,22 +20355,22 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -20384,31 +20387,31 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -20619,7 +20622,7 @@
         <v>14</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -20636,64 +20639,64 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>207</v>
@@ -20717,7 +20720,7 @@
         <v>30</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -20913,7 +20916,7 @@
         <v>40</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1766</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -20995,91 +20998,91 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1786</v>
+        <v>1787</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1788</v>
+        <v>1789</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1789</v>
+        <v>1790</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1791</v>
+        <v>1792</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>1794</v>
+        <v>1795</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1796</v>
+        <v>1797</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>1797</v>
+        <v>1798</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -21096,106 +21099,106 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1801</v>
+        <v>1802</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1802</v>
+        <v>1803</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1805</v>
+        <v>1806</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1809</v>
+        <v>1810</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1814</v>
+        <v>1815</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -21343,91 +21346,91 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -21503,7 +21506,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>912</v>
@@ -21526,13 +21529,13 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>30</v>
@@ -21552,7 +21555,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
@@ -21633,13 +21636,13 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -21656,16 +21659,16 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -21682,7 +21685,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
@@ -21777,7 +21780,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23090,7 +23093,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23181,7 +23184,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -23272,7 +23275,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>

<commit_message>
Fix duplicate instanceType bug
</commit_message>
<xml_diff>
--- a/template-generator/USDM_2.11_Test_Data_Template.xlsx
+++ b/template-generator/USDM_2.11_Test_Data_Template.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5065" uniqueCount="1890">
   <si>
     <t>Filename</t>
   </si>
@@ -6881,16 +6881,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="20" width="25.7109375" customWidth="1"/>
+    <col min="1" max="19" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -6919,37 +6919,34 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>593</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>568</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -6978,37 +6975,34 @@
         <v>598</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>600</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>30</v>
+        <v>601</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="S2" s="3" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -7046,10 +7040,10 @@
         <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>38</v>
@@ -7063,11 +7057,8 @@
       <c r="R3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -7096,37 +7087,34 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S4" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -7145,7 +7133,6 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12107,240 +12094,6 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="17" width="25.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1020</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1021</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>1022</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1024</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1026</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>1028</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>1029</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1030</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1031</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1032</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>1034</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>1035</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12376,25 +12129,25 @@
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>1020</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1021</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>14</v>
+        <v>1022</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1040</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -12411,37 +12164,37 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1041</v>
+        <v>1024</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1042</v>
+        <v>1025</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1043</v>
+        <v>1026</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1044</v>
+        <v>1027</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>1045</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>1046</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1047</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1048</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>30</v>
+        <v>1032</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1049</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -12485,10 +12238,10 @@
         <v>38</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -12517,25 +12270,25 @@
         <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>40</v>
+        <v>1034</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1034</v>
+        <v>673</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>673</v>
+        <v>779</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>779</v>
+        <v>1035</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1035</v>
+        <v>40</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>1036</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1050</v>
+        <v>755</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -12554,6 +12307,214 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="15" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13628,16 +13589,16 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="23" width="25.7109375" customWidth="1"/>
+    <col min="1" max="22" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -13666,46 +13627,43 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>1144</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1150</v>
+        <v>660</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:21">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -13734,46 +13692,43 @@
         <v>1155</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1156</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1157</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>30</v>
+        <v>1158</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1165</v>
-      </c>
-      <c r="V2" s="3" t="s">
         <v>1166</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:21">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -13811,10 +13766,10 @@
         <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>38</v>
@@ -13837,11 +13792,8 @@
       <c r="U3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -13870,46 +13822,43 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>77</v>
+        <v>1167</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>1168</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -13931,7 +13880,6 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16007,16 +15955,16 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="35" width="25.7109375" customWidth="1"/>
+    <col min="1" max="34" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -16033,94 +15981,91 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>786</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>913</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>914</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>915</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>916</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>917</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>918</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>919</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>635</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>14</v>
+        <v>1329</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1339</v>
-      </c>
-      <c r="AH1" s="1" t="s">
         <v>1340</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:33">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -16137,94 +16082,91 @@
         <v>1341</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1343</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>1349</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>1343</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>1344</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>1345</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>1346</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1347</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1348</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>1349</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1350</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1351</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1352</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>1353</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>1354</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>1355</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>1356</v>
-      </c>
       <c r="V2" s="3" t="s">
-        <v>30</v>
+        <v>1357</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1367</v>
-      </c>
-      <c r="AH2" s="3" t="s">
         <v>1368</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:33">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -16241,94 +16183,91 @@
         <v>38</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="I3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>400</v>
-      </c>
       <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AB3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34">
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -16345,94 +16284,91 @@
         <v>40</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>1008</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1016</v>
+        <v>72</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>40</v>
+        <v>1369</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1379</v>
-      </c>
-      <c r="AH4" s="3" t="s">
         <v>1380</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:33">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -16466,7 +16402,6 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18399,16 +18334,16 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:AY5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="53" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:51">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -18437,136 +18372,133 @@
         <v>462</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="AY1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:51">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -18595,136 +18527,133 @@
         <v>1638</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1639</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1640</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1641</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>1642</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1643</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>1644</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>1645</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1647</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>1648</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>1649</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>1650</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>1651</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>1652</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>1654</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>1655</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>1656</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>1657</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>1658</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>1659</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>1660</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>1661</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>1662</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>1663</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>1664</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>1665</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>1666</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>1667</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>1668</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>1669</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>1670</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>1671</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>1672</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>1673</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>1674</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>1675</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>1677</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>1678</v>
+      </c>
+      <c r="AX2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1639</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1640</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1641</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>1642</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1643</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1644</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1645</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>1646</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>1647</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>1648</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>1649</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>1650</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>1651</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>1652</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>1654</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>1655</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>1656</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>1657</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>1658</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>1659</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>1660</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>1661</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>1662</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>1663</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>1664</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>1665</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>1666</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>1667</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>1668</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>1669</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>1670</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>1671</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>1672</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>1673</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>1674</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>1675</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>1676</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>1677</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>1678</v>
-      </c>
       <c r="AY2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
         <v>1679</v>
       </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:51">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -18753,136 +18682,133 @@
         <v>39</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AC3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AH3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AN3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AP3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AR3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AS3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AT3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52">
+    </row>
+    <row r="4" spans="1:51">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -18911,136 +18837,133 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>404</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>409</v>
+        <v>550</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AV4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AW4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AN4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="AV4" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="AW4" s="3" t="s">
-        <v>560</v>
-      </c>
       <c r="AX4" s="3" t="s">
-        <v>561</v>
+        <v>40</v>
       </c>
       <c r="AY4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AZ4" s="3" t="s">
         <v>1680</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:51">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -19092,7 +19015,6 @@
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
-      <c r="AZ5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19517,16 +19439,16 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="13" width="25.7109375" customWidth="1"/>
+    <col min="1" max="12" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -19555,16 +19477,13 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -19593,16 +19512,13 @@
         <v>1687</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -19636,11 +19552,8 @@
       <c r="K3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -19669,16 +19582,13 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -19690,7 +19600,6 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20115,16 +20024,16 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="15" width="25.7109375" customWidth="1"/>
+    <col min="1" max="14" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -20153,22 +20062,19 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>1721</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1721</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>1722</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -20197,22 +20103,19 @@
         <v>1727</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1728</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
+        <v>1729</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1729</v>
-      </c>
-      <c r="N2" s="3" t="s">
         <v>1730</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -20247,16 +20150,13 @@
         <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -20285,22 +20185,19 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>40</v>
+        <v>1731</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1731</v>
-      </c>
-      <c r="N4" s="3" t="s">
         <v>1732</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -20314,7 +20211,6 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20518,16 +20414,16 @@
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="33" width="25.7109375" customWidth="1"/>
+    <col min="1" max="32" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -20556,76 +20452,73 @@
         <v>167</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="AE1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF1" s="1" t="s">
         <v>1746</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:31">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -20654,76 +20547,73 @@
         <v>1751</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1752</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1753</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1756</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>1757</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>1758</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1759</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1760</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>1761</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>1764</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1752</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1753</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1754</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>1755</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1756</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1757</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1758</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>1759</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>1760</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>1761</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>1762</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>1763</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>1765</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="AE2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF2" s="3" t="s">
         <v>1766</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:31">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -20752,76 +20642,73 @@
         <v>38</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="S3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="Y3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32">
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -20850,76 +20737,73 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>213</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>226</v>
+        <v>72</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF4" s="3" t="s">
         <v>1767</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:31">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -20951,7 +20835,6 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23495,16 +23378,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:AY5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="53" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:51">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -23533,136 +23416,133 @@
         <v>462</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="AY1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:51">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -23691,136 +23571,133 @@
         <v>508</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="AX2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>548</v>
-      </c>
       <c r="AY2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:51">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -23849,136 +23726,133 @@
         <v>39</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AC3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AH3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AN3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AP3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AR3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AS3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AT3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52">
+    </row>
+    <row r="4" spans="1:51">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -24007,136 +23881,133 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>404</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>409</v>
+        <v>550</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AV4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AW4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AN4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="AV4" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="AW4" s="3" t="s">
-        <v>560</v>
-      </c>
       <c r="AX4" s="3" t="s">
-        <v>561</v>
+        <v>40</v>
       </c>
       <c r="AY4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AZ4" s="3" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:51">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -24188,7 +24059,6 @@
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
-      <c r="AZ5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24197,16 +24067,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="20" width="25.7109375" customWidth="1"/>
+    <col min="1" max="19" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -24235,37 +24105,34 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>568</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -24294,37 +24161,34 @@
         <v>579</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>580</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
+        <v>581</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="S2" s="3" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -24359,31 +24223,28 @@
         <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -24412,37 +24273,34 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="S4" s="3" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -24461,7 +24319,6 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
389 create new test template for core usdm v30 (#178)
* Updates for 2.11 template and readme, add 3.0 template (copy of 2.11)

* Fix duplicate instanceType bug
</commit_message>
<xml_diff>
--- a/template-generator/USDM_2.11_Test_Data_Template.xlsx
+++ b/template-generator/USDM_2.11_Test_Data_Template.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="1890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5065" uniqueCount="1890">
   <si>
     <t>Filename</t>
   </si>
@@ -6881,16 +6881,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="20" width="25.7109375" customWidth="1"/>
+    <col min="1" max="19" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -6919,37 +6919,34 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>593</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>568</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -6978,37 +6975,34 @@
         <v>598</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>600</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>30</v>
+        <v>601</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="S2" s="3" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -7046,10 +7040,10 @@
         <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>38</v>
@@ -7063,11 +7057,8 @@
       <c r="R3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -7096,37 +7087,34 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S4" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -7145,7 +7133,6 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12107,240 +12094,6 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="17" width="25.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1020</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1021</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>1022</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1024</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1026</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>1028</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>1029</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1030</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1031</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1032</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>1034</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>1035</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12376,25 +12129,25 @@
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>1020</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1021</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>14</v>
+        <v>1022</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1040</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -12411,37 +12164,37 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1041</v>
+        <v>1024</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1042</v>
+        <v>1025</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1043</v>
+        <v>1026</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1044</v>
+        <v>1027</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>1045</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>1046</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1047</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1048</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>30</v>
+        <v>1032</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1049</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -12485,10 +12238,10 @@
         <v>38</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -12517,25 +12270,25 @@
         <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>40</v>
+        <v>1034</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1034</v>
+        <v>673</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>673</v>
+        <v>779</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>779</v>
+        <v>1035</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1035</v>
+        <v>40</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>1036</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1050</v>
+        <v>755</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -12554,6 +12307,214 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="15" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13628,16 +13589,16 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="23" width="25.7109375" customWidth="1"/>
+    <col min="1" max="22" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -13666,46 +13627,43 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>1144</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1150</v>
+        <v>660</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:21">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -13734,46 +13692,43 @@
         <v>1155</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1156</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1157</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>30</v>
+        <v>1158</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>1165</v>
-      </c>
-      <c r="V2" s="3" t="s">
         <v>1166</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:21">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -13811,10 +13766,10 @@
         <v>38</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>38</v>
@@ -13837,11 +13792,8 @@
       <c r="U3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -13870,46 +13822,43 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>77</v>
+        <v>1167</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>1168</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -13931,7 +13880,6 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16007,16 +15955,16 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="35" width="25.7109375" customWidth="1"/>
+    <col min="1" max="34" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -16033,94 +15981,91 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>786</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>913</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>914</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>915</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>916</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>917</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>918</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>919</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>635</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>14</v>
+        <v>1329</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>1339</v>
-      </c>
-      <c r="AH1" s="1" t="s">
         <v>1340</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:33">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -16137,94 +16082,91 @@
         <v>1341</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1343</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>1349</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>1343</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>1344</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>1345</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>1346</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1347</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1348</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>1349</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1350</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1351</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1352</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>1353</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>1354</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>1355</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>1356</v>
-      </c>
       <c r="V2" s="3" t="s">
-        <v>30</v>
+        <v>1357</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>1367</v>
-      </c>
-      <c r="AH2" s="3" t="s">
         <v>1368</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:33">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -16241,94 +16183,91 @@
         <v>38</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="I3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>400</v>
-      </c>
       <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AB3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34">
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -16345,94 +16284,91 @@
         <v>40</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>1008</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1016</v>
+        <v>72</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>40</v>
+        <v>1369</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>1379</v>
-      </c>
-      <c r="AH4" s="3" t="s">
         <v>1380</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:33">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -16466,7 +16402,6 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18399,16 +18334,16 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:AY5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="53" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:51">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -18437,136 +18372,133 @@
         <v>462</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="AY1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:51">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -18595,136 +18527,133 @@
         <v>1638</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1639</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1640</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1641</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>1642</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1643</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>1644</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>1645</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1647</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>1648</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>1649</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>1650</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>1651</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>1652</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>1654</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>1655</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>1656</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>1657</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>1658</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>1659</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>1660</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>1661</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>1662</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>1663</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>1664</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>1665</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>1666</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>1667</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>1668</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>1669</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>1670</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>1671</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>1672</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>1673</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>1674</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>1675</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>1677</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>1678</v>
+      </c>
+      <c r="AX2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1639</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1640</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1641</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>1642</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1643</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1644</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1645</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>1646</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>1647</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>1648</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>1649</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>1650</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>1651</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>1652</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>1654</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>1655</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>1656</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>1657</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>1658</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>1659</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>1660</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>1661</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>1662</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>1663</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>1664</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>1665</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>1666</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>1667</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>1668</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>1669</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>1670</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>1671</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>1672</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>1673</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>1674</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>1675</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>1676</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>1677</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>1678</v>
-      </c>
       <c r="AY2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
         <v>1679</v>
       </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:51">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -18753,136 +18682,133 @@
         <v>39</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AC3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AH3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AN3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AP3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AR3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AS3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AT3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52">
+    </row>
+    <row r="4" spans="1:51">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -18911,136 +18837,133 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>404</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>409</v>
+        <v>550</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AV4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AW4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AN4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="AV4" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="AW4" s="3" t="s">
-        <v>560</v>
-      </c>
       <c r="AX4" s="3" t="s">
-        <v>561</v>
+        <v>40</v>
       </c>
       <c r="AY4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AZ4" s="3" t="s">
         <v>1680</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:51">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -19092,7 +19015,6 @@
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
-      <c r="AZ5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19517,16 +19439,16 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="13" width="25.7109375" customWidth="1"/>
+    <col min="1" max="12" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -19555,16 +19477,13 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -19593,16 +19512,13 @@
         <v>1687</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -19636,11 +19552,8 @@
       <c r="K3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -19669,16 +19582,13 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -19690,7 +19600,6 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20115,16 +20024,16 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="15" width="25.7109375" customWidth="1"/>
+    <col min="1" max="14" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -20153,22 +20062,19 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>1721</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1721</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>1722</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -20197,22 +20103,19 @@
         <v>1727</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1728</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
+        <v>1729</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1729</v>
-      </c>
-      <c r="N2" s="3" t="s">
         <v>1730</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -20247,16 +20150,13 @@
         <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -20285,22 +20185,19 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>40</v>
+        <v>1731</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>1731</v>
-      </c>
-      <c r="N4" s="3" t="s">
         <v>1732</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -20314,7 +20211,6 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20518,16 +20414,16 @@
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="33" width="25.7109375" customWidth="1"/>
+    <col min="1" max="32" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -20556,76 +20452,73 @@
         <v>167</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="AE1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF1" s="1" t="s">
         <v>1746</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:31">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -20654,76 +20547,73 @@
         <v>1751</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>1752</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1753</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1756</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>1757</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>1758</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1759</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1760</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>1761</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>1762</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>1764</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>1752</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>1753</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1754</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>1755</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1756</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1757</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1758</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>1759</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>1760</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>1761</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>1762</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>1763</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>1764</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>1765</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="AE2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF2" s="3" t="s">
         <v>1766</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:31">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -20752,76 +20642,73 @@
         <v>38</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="S3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="Y3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32">
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -20850,76 +20737,73 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>213</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>226</v>
+        <v>72</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF4" s="3" t="s">
         <v>1767</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:31">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -20951,7 +20835,6 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23495,16 +23378,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:AY5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="53" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:51">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -23533,136 +23416,133 @@
         <v>462</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="AY1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:51">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -23691,136 +23571,133 @@
         <v>508</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="AX2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>548</v>
-      </c>
       <c r="AY2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:51">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -23849,136 +23726,133 @@
         <v>39</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AC3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AH3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AN3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="AP3" s="3" t="s">
         <v>400</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>400</v>
+        <v>39</v>
       </c>
       <c r="AR3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AS3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AT3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52">
+    </row>
+    <row r="4" spans="1:51">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -24007,136 +23881,133 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>404</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>409</v>
+        <v>550</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AV4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AW4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AN4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="AV4" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="AW4" s="3" t="s">
-        <v>560</v>
-      </c>
       <c r="AX4" s="3" t="s">
-        <v>561</v>
+        <v>40</v>
       </c>
       <c r="AY4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AZ4" s="3" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:51">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -24188,7 +24059,6 @@
       <c r="AW5" s="4"/>
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
-      <c r="AZ5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24197,16 +24067,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="20" width="25.7109375" customWidth="1"/>
+    <col min="1" max="19" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -24235,37 +24105,34 @@
         <v>566</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>567</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>568</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -24294,37 +24161,34 @@
         <v>579</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>580</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
+        <v>581</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="S2" s="3" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -24359,31 +24223,28 @@
         <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -24412,37 +24273,34 @@
         <v>40</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>588</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>588</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="S4" s="3" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -24461,7 +24319,6 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>